<commit_message>
new versions 17 jan 22
</commit_message>
<xml_diff>
--- a/DATAofStoryBotHelper.xlsx
+++ b/DATAofStoryBotHelper.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Темы</t>
   </si>
@@ -79,11 +79,14 @@
   <si>
     <t>Сыллка на тест2</t>
   </si>
+  <si>
+    <t>тема2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -125,14 +128,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -170,9 +176,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,7 +213,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,6 +570,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -578,6 +587,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -591,6 +603,23 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>